<commit_message>
Uzlabots Testēšanas žurnals, to saturs
</commit_message>
<xml_diff>
--- a/Testa_Zurnals_Zeiburlins.xlsx
+++ b/Testa_Zurnals_Zeiburlins.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karli\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karli\Desktop\Files\C++ tips\darbini\testa_kods\Eksamena_darbs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDE03DB-DC81-4A28-9B8E-543F84979270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85A1DA0-D9B2-4727-B401-F589BDC08DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{93516470-F0EC-41B1-83D0-5F7F7FFCE06E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{93516470-F0EC-41B1-83D0-5F7F7FFCE06E}"/>
   </bookViews>
   <sheets>
     <sheet name="Aprkasts" sheetId="1" r:id="rId1"/>
     <sheet name="Prasības" sheetId="2" r:id="rId2"/>
     <sheet name="Testa piemeri" sheetId="3" r:id="rId3"/>
+    <sheet name="Testēšanas žurnāls" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="200">
   <si>
     <t>Identifikatoru atšifrējums</t>
   </si>
@@ -147,12 +148,6 @@
   </si>
   <si>
     <t>PR.JAU.10</t>
-  </si>
-  <si>
-    <t>PAZ</t>
-  </si>
-  <si>
-    <t>Pazinojuma izvade</t>
   </si>
   <si>
     <t>Jautajumi un atbildes</t>
@@ -219,9 +214,6 @@
 Peles kreisais taustiņš</t>
   </si>
   <si>
-    <t xml:space="preserve">Tieks aizvērta programma </t>
-  </si>
-  <si>
     <t>TP.JAU.01</t>
   </si>
   <si>
@@ -440,9 +432,6 @@
     <t>TP.NA.10</t>
   </si>
   <si>
-    <t>Atbilde uz jautājumu</t>
-  </si>
-  <si>
     <t>TP.REZ.01</t>
   </si>
   <si>
@@ -474,13 +463,184 @@
   </si>
   <si>
     <t>Tieks izvadits iegūto punktu skaits un jautajumi uz kuriem atbildets nepareizi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiek aizvērta programma </t>
+  </si>
+  <si>
+    <t>Testēšanas ID</t>
+  </si>
+  <si>
+    <t>Datums</t>
+  </si>
+  <si>
+    <t>Testpiemēra ID</t>
+  </si>
+  <si>
+    <t>Testpiemēra nosaukums</t>
+  </si>
+  <si>
+    <t>Testētājs</t>
+  </si>
+  <si>
+    <t>Statuss</t>
+  </si>
+  <si>
+    <t>Kļūdas ziņojums</t>
+  </si>
+  <si>
+    <t>Kļūdas ziņojuma Nr.</t>
+  </si>
+  <si>
+    <t>TZ</t>
+  </si>
+  <si>
+    <t>Testēšanas žurnals</t>
+  </si>
+  <si>
+    <t>TZ.01</t>
+  </si>
+  <si>
+    <t>Kārlis Zeiburliņš</t>
+  </si>
+  <si>
+    <t>TZ.02</t>
+  </si>
+  <si>
+    <t>TZ.03</t>
+  </si>
+  <si>
+    <t>TZ.04</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz jautājumu Nr.1</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz jautājumu Nr.1</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz jautājumu Nr.2</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz jautājumu Nr.2</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz jautājumu Nr.3</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz jautājumu Nr.3</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz jautājumu Nr.4</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz jautājumu Nr.4</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz jautājumu Nr.5</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz jautājumu Nr.5</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz jautājumu Nr.6</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz jautājumu Nr.6</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz jautājumu Nr.7</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz jautājumu Nr.7</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz jautājumu Nr.8</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz jautājumu Nr.8</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz jautājumu Nr.9</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz jautājumu Nr.9</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz jautājumu Nr.10</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz jautājumu Nr.10</t>
+  </si>
+  <si>
+    <t>TZ.05</t>
+  </si>
+  <si>
+    <t>TZ.06</t>
+  </si>
+  <si>
+    <t>TZ.07</t>
+  </si>
+  <si>
+    <t>TZ.08</t>
+  </si>
+  <si>
+    <t>TZ.09</t>
+  </si>
+  <si>
+    <t>TZ.10</t>
+  </si>
+  <si>
+    <t>TZ.11</t>
+  </si>
+  <si>
+    <t>TZ.12</t>
+  </si>
+  <si>
+    <t>TZ.13</t>
+  </si>
+  <si>
+    <t>TZ.14</t>
+  </si>
+  <si>
+    <t>TZ.15</t>
+  </si>
+  <si>
+    <t>TZ.16</t>
+  </si>
+  <si>
+    <t>TZ.17</t>
+  </si>
+  <si>
+    <t>TZ.18</t>
+  </si>
+  <si>
+    <t>TZ.19</t>
+  </si>
+  <si>
+    <t>TZ.20</t>
+  </si>
+  <si>
+    <t>TZ.21</t>
+  </si>
+  <si>
+    <t>TZ.22</t>
+  </si>
+  <si>
+    <t>TZ.23</t>
+  </si>
+  <si>
+    <t>TZ.24</t>
+  </si>
+  <si>
+    <t>Veiksmīgs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,8 +733,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -599,6 +774,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="29">
     <border>
@@ -978,7 +1159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1001,39 +1182,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1080,9 +1228,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1094,6 +1239,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1103,50 +1326,107 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1465,19 +1745,19 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1487,22 +1767,22 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -1534,22 +1814,22 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="20"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
@@ -1557,10 +1837,10 @@
       <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="19"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
@@ -1568,10 +1848,10 @@
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="19"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
@@ -1579,10 +1859,10 @@
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="19"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
@@ -1590,16 +1870,16 @@
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="14"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>41</v>
@@ -1610,12 +1890,11 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="4"/>
+        <v>152</v>
+      </c>
+      <c r="B15" t="s">
+        <v>153</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
@@ -1713,7 +1992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CF6A77-FDCF-4E41-A527-815496E8B293}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
@@ -1732,208 +2011,208 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="22"/>
+      <c r="B2" s="52"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="22"/>
+      <c r="A6" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="52"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="26"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C10" s="8"/>
-      <c r="D10" s="26"/>
+      <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="26"/>
+        <v>87</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="26"/>
+      <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="26"/>
+        <v>90</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="26"/>
+      <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="26"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="15"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C16" s="8"/>
-      <c r="D16" s="26"/>
+      <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="26"/>
+        <v>93</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="15"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="26"/>
+      <c r="D18" s="15"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="26"/>
+        <v>95</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="26"/>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C22" s="8"/>
-      <c r="D22" s="26"/>
+      <c r="D22" s="15"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="26"/>
+        <v>99</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="15"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="26"/>
+      <c r="D24" s="15"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="26"/>
+        <v>101</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="26"/>
+      <c r="D26" s="15"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
@@ -1944,15 +2223,15 @@
         <v>37</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1964,15 +2243,15 @@
         <v>38</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1984,42 +2263,42 @@
         <v>39</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="24"/>
+      <c r="A36" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="54"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="21"/>
-      <c r="B39" s="22"/>
+      <c r="A39" s="51"/>
+      <c r="B39" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2038,8 +2317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8C0C11-0FD4-4A5B-96C5-5DDF38298718}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2050,816 +2329,1554 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="19" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="63"/>
+    </row>
+    <row r="3" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="57"/>
+    </row>
+    <row r="5" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="57"/>
+    </row>
+    <row r="7" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
-    </row>
-    <row r="3" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" s="39" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="52"/>
-    </row>
-    <row r="5" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="38" t="s">
+      <c r="E7" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="G8" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="55"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="57"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="B10" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="55"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="57"/>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="40" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="52"/>
-    </row>
-    <row r="7" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="B13" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="55"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="57"/>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B16" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="55"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="57"/>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="55"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="57"/>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="55"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="57"/>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="G25" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H26" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="55"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="57"/>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="F28" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H28" s="34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="55"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="57"/>
+    </row>
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="G31" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H31" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H32" s="24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="55"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="57"/>
+    </row>
+    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="G34" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H34" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H35" s="24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="58"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="60"/>
+    </row>
+    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="E37" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="G7" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="46" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" s="35" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50"/>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="52"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="F10" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="G10" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="46" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="52"/>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C13" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="G13" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="H13" s="46" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="B14" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="F14" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="G14" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H14" s="35" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="50"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="52"/>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C16" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="F16" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G16" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="H16" s="46" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="B17" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="F17" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="G17" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" s="35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="50"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="52"/>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C19" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="F19" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G19" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="H19" s="46" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="F20" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="G20" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H20" s="35" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="52"/>
-    </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C22" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G22" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="H22" s="46" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="B23" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C23" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="F23" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="G23" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H23" s="35" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="50"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="52"/>
-    </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C25" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G25" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="H25" s="46" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="B26" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="F26" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="G26" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H26" s="35" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="50"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="52"/>
-    </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C28" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="D28" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="E28" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="F28" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G28" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="H28" s="46" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="B29" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D29" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="F29" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="G29" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H29" s="35" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="50"/>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="52"/>
-    </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C31" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="E31" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="F31" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G31" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="H31" s="46" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="31" t="s">
+      <c r="F37" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="G37" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="H37" s="39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="B32" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C32" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D32" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="E32" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="F32" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="G32" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H32" s="35" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="50"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="52"/>
-    </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C34" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="E34" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="F34" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G34" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="H34" s="46" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="B35" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="E35" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="F35" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="G35" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H35" s="35" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="53"/>
-      <c r="B36" s="54"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="55"/>
-    </row>
-    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="56" t="s">
+      <c r="D38" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="E38" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="F38" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="B37" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="58" t="s">
-        <v>137</v>
-      </c>
-      <c r="D37" s="58" t="s">
-        <v>138</v>
-      </c>
-      <c r="E37" s="58" t="s">
-        <v>139</v>
-      </c>
-      <c r="F37" s="59" t="s">
-        <v>140</v>
-      </c>
-      <c r="G37" s="58" t="s">
-        <v>141</v>
-      </c>
-      <c r="H37" s="60" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="61" t="s">
+      <c r="G38" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="B38" s="62" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38" s="62" t="s">
-        <v>137</v>
-      </c>
-      <c r="D38" s="62" t="s">
-        <v>143</v>
-      </c>
-      <c r="E38" s="62" t="s">
-        <v>145</v>
-      </c>
-      <c r="F38" s="63" t="s">
-        <v>140</v>
-      </c>
-      <c r="G38" s="62" t="s">
-        <v>146</v>
-      </c>
-      <c r="H38" s="64" t="s">
-        <v>46</v>
+      <c r="H38" s="43" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="50"/>
-      <c r="B39" s="51"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="51"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="51"/>
-      <c r="H39" s="52"/>
+      <c r="A39" s="55"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A21:H21"/>
     <mergeCell ref="A39:H39"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="A30:H30"/>
     <mergeCell ref="A33:H33"/>
     <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A2:H2"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E748FC68-B45F-4508-A7C1-F644815860A2}">
+  <dimension ref="A1:H39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="52.85546875" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="74" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="67"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="84" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="85">
+        <v>44364</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="86" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="87" t="s">
+        <v>199</v>
+      </c>
+      <c r="G3" s="86"/>
+      <c r="H3" s="88"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="71"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="84" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="85">
+        <v>44364</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="86" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" s="87" t="s">
+        <v>199</v>
+      </c>
+      <c r="G5" s="86"/>
+      <c r="H5" s="88"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="69"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="71"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="89" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7" s="90">
+        <v>44364</v>
+      </c>
+      <c r="C7" s="91" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="64" t="s">
+        <v>159</v>
+      </c>
+      <c r="E7" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="F7" s="93" t="s">
+        <v>199</v>
+      </c>
+      <c r="G7" s="92"/>
+      <c r="H7" s="94"/>
+    </row>
+    <row r="8" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="75" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="76">
+        <v>44364</v>
+      </c>
+      <c r="C8" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="81" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="78" t="s">
+        <v>155</v>
+      </c>
+      <c r="F8" s="79" t="s">
+        <v>199</v>
+      </c>
+      <c r="G8" s="78"/>
+      <c r="H8" s="80"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="69"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="71"/>
+    </row>
+    <row r="10" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="89" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" s="90">
+        <v>44364</v>
+      </c>
+      <c r="C10" s="91" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="64" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" s="93" t="s">
+        <v>199</v>
+      </c>
+      <c r="G10" s="92"/>
+      <c r="H10" s="94"/>
+    </row>
+    <row r="11" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="75" t="s">
+        <v>180</v>
+      </c>
+      <c r="B11" s="76">
+        <v>44364</v>
+      </c>
+      <c r="C11" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="81" t="s">
+        <v>162</v>
+      </c>
+      <c r="E11" s="78" t="s">
+        <v>155</v>
+      </c>
+      <c r="F11" s="79" t="s">
+        <v>199</v>
+      </c>
+      <c r="G11" s="78"/>
+      <c r="H11" s="80"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="69"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="71"/>
+    </row>
+    <row r="13" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="89" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="90">
+        <v>44364</v>
+      </c>
+      <c r="C13" s="91" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="F13" s="93" t="s">
+        <v>199</v>
+      </c>
+      <c r="G13" s="92"/>
+      <c r="H13" s="94"/>
+    </row>
+    <row r="14" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="75" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="76">
+        <v>44364</v>
+      </c>
+      <c r="C14" s="77" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="81" t="s">
+        <v>164</v>
+      </c>
+      <c r="E14" s="78" t="s">
+        <v>155</v>
+      </c>
+      <c r="F14" s="79" t="s">
+        <v>199</v>
+      </c>
+      <c r="G14" s="78"/>
+      <c r="H14" s="80"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="69"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="71"/>
+    </row>
+    <row r="16" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="95" t="s">
+        <v>183</v>
+      </c>
+      <c r="B16" s="90">
+        <v>44364</v>
+      </c>
+      <c r="C16" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="64" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="F16" s="93" t="s">
+        <v>199</v>
+      </c>
+      <c r="G16" s="92"/>
+      <c r="H16" s="94"/>
+    </row>
+    <row r="17" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="82" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17" s="76">
+        <v>44364</v>
+      </c>
+      <c r="C17" s="77" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="81" t="s">
+        <v>166</v>
+      </c>
+      <c r="E17" s="78" t="s">
+        <v>155</v>
+      </c>
+      <c r="F17" s="79" t="s">
+        <v>199</v>
+      </c>
+      <c r="G17" s="78"/>
+      <c r="H17" s="80"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="69"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="71"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="95" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" s="90">
+        <v>44364</v>
+      </c>
+      <c r="C19" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="F19" s="93" t="s">
+        <v>199</v>
+      </c>
+      <c r="G19" s="92"/>
+      <c r="H19" s="94"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="82" t="s">
+        <v>186</v>
+      </c>
+      <c r="B20" s="76">
+        <v>44364</v>
+      </c>
+      <c r="C20" s="77" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="81" t="s">
+        <v>168</v>
+      </c>
+      <c r="E20" s="78" t="s">
+        <v>155</v>
+      </c>
+      <c r="F20" s="79" t="s">
+        <v>199</v>
+      </c>
+      <c r="G20" s="78"/>
+      <c r="H20" s="80"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="69"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="71"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="95" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22" s="90">
+        <v>44364</v>
+      </c>
+      <c r="C22" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="64" t="s">
+        <v>169</v>
+      </c>
+      <c r="E22" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="F22" s="93" t="s">
+        <v>199</v>
+      </c>
+      <c r="G22" s="92"/>
+      <c r="H22" s="94"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="82" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" s="76">
+        <v>44364</v>
+      </c>
+      <c r="C23" s="77" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="81" t="s">
+        <v>170</v>
+      </c>
+      <c r="E23" s="78" t="s">
+        <v>155</v>
+      </c>
+      <c r="F23" s="79" t="s">
+        <v>199</v>
+      </c>
+      <c r="G23" s="78"/>
+      <c r="H23" s="80"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="69"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="71"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="95" t="s">
+        <v>189</v>
+      </c>
+      <c r="B25" s="96">
+        <v>44364</v>
+      </c>
+      <c r="C25" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="64" t="s">
+        <v>171</v>
+      </c>
+      <c r="E25" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="F25" s="93" t="s">
+        <v>199</v>
+      </c>
+      <c r="G25" s="92"/>
+      <c r="H25" s="94"/>
+    </row>
+    <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="82" t="s">
+        <v>190</v>
+      </c>
+      <c r="B26" s="76">
+        <v>44364</v>
+      </c>
+      <c r="C26" s="77" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="81" t="s">
+        <v>172</v>
+      </c>
+      <c r="E26" s="78" t="s">
+        <v>155</v>
+      </c>
+      <c r="F26" s="79" t="s">
+        <v>199</v>
+      </c>
+      <c r="G26" s="78"/>
+      <c r="H26" s="80"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="69"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="71"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="95" t="s">
+        <v>191</v>
+      </c>
+      <c r="B28" s="90">
+        <v>44364</v>
+      </c>
+      <c r="C28" s="91" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="64" t="s">
+        <v>173</v>
+      </c>
+      <c r="E28" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="F28" s="93" t="s">
+        <v>199</v>
+      </c>
+      <c r="G28" s="92"/>
+      <c r="H28" s="94"/>
+    </row>
+    <row r="29" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="82" t="s">
+        <v>192</v>
+      </c>
+      <c r="B29" s="76">
+        <v>44364</v>
+      </c>
+      <c r="C29" s="77" t="s">
+        <v>129</v>
+      </c>
+      <c r="D29" s="81" t="s">
+        <v>174</v>
+      </c>
+      <c r="E29" s="78" t="s">
+        <v>155</v>
+      </c>
+      <c r="F29" s="79" t="s">
+        <v>199</v>
+      </c>
+      <c r="G29" s="78"/>
+      <c r="H29" s="80"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="69"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="71"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="95" t="s">
+        <v>193</v>
+      </c>
+      <c r="B31" s="90">
+        <v>44364</v>
+      </c>
+      <c r="C31" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="64" t="s">
+        <v>175</v>
+      </c>
+      <c r="E31" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="F31" s="93" t="s">
+        <v>199</v>
+      </c>
+      <c r="G31" s="92"/>
+      <c r="H31" s="94"/>
+    </row>
+    <row r="32" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="82" t="s">
+        <v>194</v>
+      </c>
+      <c r="B32" s="76">
+        <v>44364</v>
+      </c>
+      <c r="C32" s="77" t="s">
+        <v>130</v>
+      </c>
+      <c r="D32" s="81" t="s">
+        <v>176</v>
+      </c>
+      <c r="E32" s="78" t="s">
+        <v>155</v>
+      </c>
+      <c r="F32" s="79" t="s">
+        <v>199</v>
+      </c>
+      <c r="G32" s="78"/>
+      <c r="H32" s="80"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="69"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="71"/>
+    </row>
+    <row r="34" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="95" t="s">
+        <v>195</v>
+      </c>
+      <c r="B34" s="90">
+        <v>44364</v>
+      </c>
+      <c r="C34" s="91" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="E34" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="F34" s="93" t="s">
+        <v>199</v>
+      </c>
+      <c r="G34" s="92"/>
+      <c r="H34" s="94"/>
+    </row>
+    <row r="35" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="82" t="s">
+        <v>196</v>
+      </c>
+      <c r="B35" s="76">
+        <v>44364</v>
+      </c>
+      <c r="C35" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" s="81" t="s">
+        <v>178</v>
+      </c>
+      <c r="E35" s="78" t="s">
+        <v>155</v>
+      </c>
+      <c r="F35" s="79" t="s">
+        <v>199</v>
+      </c>
+      <c r="G35" s="78"/>
+      <c r="H35" s="80"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="69"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="70"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="71"/>
+    </row>
+    <row r="37" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="95" t="s">
+        <v>197</v>
+      </c>
+      <c r="B37" s="90">
+        <v>44364</v>
+      </c>
+      <c r="C37" s="91" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="97" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="F37" s="93" t="s">
+        <v>199</v>
+      </c>
+      <c r="G37" s="92"/>
+      <c r="H37" s="94"/>
+    </row>
+    <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="82" t="s">
+        <v>198</v>
+      </c>
+      <c r="B38" s="76">
+        <v>44364</v>
+      </c>
+      <c r="C38" s="77" t="s">
+        <v>138</v>
+      </c>
+      <c r="D38" s="83" t="s">
+        <v>140</v>
+      </c>
+      <c r="E38" s="78" t="s">
+        <v>155</v>
+      </c>
+      <c r="F38" s="79" t="s">
+        <v>199</v>
+      </c>
+      <c r="G38" s="78"/>
+      <c r="H38" s="80"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="69"/>
+      <c r="B39" s="70"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="71"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A39:H39"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A12:H12"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Veicu uzlabojumu Testa žurnālā
</commit_message>
<xml_diff>
--- a/Testa_Zurnals_Zeiburlins.xlsx
+++ b/Testa_Zurnals_Zeiburlins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karli\Desktop\Files\C++ tips\darbini\testa_kods\Eksamena_darbs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C15943-5883-42C1-A0CD-3CDFDF22D1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F7C5E0-BDB3-45D7-B3A0-79E7C7C80707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{93516470-F0EC-41B1-83D0-5F7F7FFCE06E}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="199">
   <si>
     <t>Identifikatoru atšifrējums</t>
   </si>
@@ -114,42 +114,9 @@
     <t>Programmas „Tests_Zeiburlins” aizvēršana</t>
   </si>
   <si>
-    <t>JAU</t>
-  </si>
-  <si>
-    <t>Jautājums</t>
-  </si>
-  <si>
-    <t>PR.JAU.01</t>
-  </si>
-  <si>
-    <t>PR.JAU.02</t>
-  </si>
-  <si>
-    <t>PR.JAU.03</t>
-  </si>
-  <si>
-    <t>PR.JAU.04</t>
-  </si>
-  <si>
-    <t>PR.JAU.05</t>
-  </si>
-  <si>
-    <t>PR.JAU.06</t>
-  </si>
-  <si>
-    <t>PR.JAU.07</t>
-  </si>
-  <si>
     <t>PR.JAU.08</t>
   </si>
   <si>
-    <t>PR.JAU.09</t>
-  </si>
-  <si>
-    <t>PR.JAU.10</t>
-  </si>
-  <si>
     <t>Jautajumi un atbildes</t>
   </si>
   <si>
@@ -199,36 +166,6 @@
   </si>
   <si>
     <t>Programmas izslēgšana uz Windows darbstacijas</t>
-  </si>
-  <si>
-    <t>TP.JAU.01</t>
-  </si>
-  <si>
-    <t>TP.JAU.02</t>
-  </si>
-  <si>
-    <t>TP.JAU.03</t>
-  </si>
-  <si>
-    <t>TP.JAU.04</t>
-  </si>
-  <si>
-    <t>TP.JAU.05</t>
-  </si>
-  <si>
-    <t>TP.JAU.06</t>
-  </si>
-  <si>
-    <t>TP.JAU.07</t>
-  </si>
-  <si>
-    <t>TP.JAU.08</t>
-  </si>
-  <si>
-    <t>TP.JAU.09</t>
-  </si>
-  <si>
-    <t>TP.JAU.10</t>
   </si>
   <si>
     <t>Black Box</t>
@@ -633,6 +570,66 @@
   <si>
     <t>Peles kreisā taustiņa dubultklikšķis
 Peles kreisais taustiņš</t>
+  </si>
+  <si>
+    <t>PR.PA.01</t>
+  </si>
+  <si>
+    <t>PR.PA.02</t>
+  </si>
+  <si>
+    <t>PR.PA.03</t>
+  </si>
+  <si>
+    <t>PR.PA.04</t>
+  </si>
+  <si>
+    <t>PR.PA.05</t>
+  </si>
+  <si>
+    <t>PR.PA.06</t>
+  </si>
+  <si>
+    <t>PR.PA.07</t>
+  </si>
+  <si>
+    <t>PR.PA.08</t>
+  </si>
+  <si>
+    <t>PR.PA.09</t>
+  </si>
+  <si>
+    <t>PR.PA.10</t>
+  </si>
+  <si>
+    <t>TP.PA.01</t>
+  </si>
+  <si>
+    <t>TP.PA.02</t>
+  </si>
+  <si>
+    <t>TP.PA.03</t>
+  </si>
+  <si>
+    <t>TP.PA.04</t>
+  </si>
+  <si>
+    <t>TP.PA.05</t>
+  </si>
+  <si>
+    <t>TP.PA.06</t>
+  </si>
+  <si>
+    <t>TP.PA.07</t>
+  </si>
+  <si>
+    <t>TP.PA.08</t>
+  </si>
+  <si>
+    <t>TP.PA.09</t>
+  </si>
+  <si>
+    <t>TP.PA.10</t>
   </si>
 </sst>
 </file>
@@ -1158,7 +1155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1343,15 +1340,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1391,6 +1382,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1400,14 +1400,14 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1418,14 +1418,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1744,19 +1738,19 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1766,22 +1760,22 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -1813,22 +1807,22 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="78" t="s">
+      <c r="B9" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="78"/>
+      <c r="C9" s="76"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
@@ -1836,10 +1830,10 @@
       <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="77"/>
+      <c r="C10" s="75"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
@@ -1847,10 +1841,10 @@
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="77"/>
+      <c r="C11" s="75"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
@@ -1858,42 +1852,35 @@
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="77" t="s">
+      <c r="B12" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="77"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="72" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="72"/>
+        <v>31</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="4"/>
+        <v>127</v>
+      </c>
+      <c r="B14" t="s">
+        <v>128</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B15" t="s">
-        <v>149</v>
-      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
@@ -1971,8 +1958,7 @@
       <c r="A26" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B13:C13"/>
+  <mergeCells count="8">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
@@ -1991,8 +1977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CF6A77-FDCF-4E41-A527-815496E8B293}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2010,51 +1996,51 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="80"/>
+      <c r="B2" s="78"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="79"/>
-      <c r="B4" s="80"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="79" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="80"/>
+      <c r="A6" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="78"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>30</v>
+        <v>179</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2065,20 +2051,20 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>31</v>
+        <v>180</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="15"/>
@@ -2091,20 +2077,20 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>32</v>
+        <v>181</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="15"/>
@@ -2117,20 +2103,20 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>33</v>
+        <v>182</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="15"/>
@@ -2143,20 +2129,20 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>34</v>
+        <v>183</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="15"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="15"/>
@@ -2169,20 +2155,20 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>35</v>
+        <v>184</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="15"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="15"/>
@@ -2195,20 +2181,20 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>36</v>
+        <v>185</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="15"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="15"/>
@@ -2219,18 +2205,18 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>37</v>
+        <v>186</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2239,18 +2225,18 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>38</v>
+        <v>187</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2259,45 +2245,45 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>39</v>
+        <v>188</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="81" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" s="82"/>
+      <c r="A36" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="80"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="79"/>
-      <c r="B39" s="80"/>
+      <c r="A39" s="77"/>
+      <c r="B39" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2317,7 +2303,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2354,773 +2340,778 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="86" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="88"/>
+      <c r="A2" s="87" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="89"/>
     </row>
     <row r="3" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="83"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="85"/>
+      <c r="A4" s="81"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="83"/>
     </row>
     <row r="5" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="83"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="85"/>
+      <c r="A6" s="81"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="83"/>
     </row>
     <row r="7" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
-        <v>57</v>
+        <v>189</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="H7" s="34" t="s">
-        <v>30</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="83"/>
-      <c r="B9" s="84"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="85"/>
+      <c r="A9" s="81"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="83"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>58</v>
+        <v>190</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="H10" s="34" t="s">
-        <v>31</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="83"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="85"/>
+      <c r="A12" s="81"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="83"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
-        <v>59</v>
+        <v>191</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>32</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="83"/>
-      <c r="B15" s="84"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="85"/>
+      <c r="A15" s="81"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="83"/>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
-        <v>60</v>
+        <v>192</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>33</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="83"/>
-      <c r="B18" s="84"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="85"/>
+      <c r="A18" s="81"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="82"/>
+      <c r="G18" s="82"/>
+      <c r="H18" s="83"/>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>61</v>
+        <v>193</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="H19" s="34" t="s">
-        <v>34</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="G20" s="21" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="83"/>
-      <c r="B21" s="84"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="84"/>
-      <c r="F21" s="84"/>
-      <c r="G21" s="84"/>
-      <c r="H21" s="85"/>
+      <c r="A21" s="81"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="82"/>
+      <c r="G21" s="82"/>
+      <c r="H21" s="83"/>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
-        <v>62</v>
+        <v>194</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="G22" s="32" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="H22" s="34" t="s">
-        <v>35</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="83"/>
-      <c r="B24" s="84"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="84"/>
-      <c r="G24" s="84"/>
-      <c r="H24" s="85"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="83"/>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
-        <v>63</v>
+        <v>195</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E25" s="32" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="F25" s="33" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="G25" s="32" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="H25" s="34" t="s">
-        <v>36</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="20" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="F26" s="23" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="83"/>
-      <c r="B27" s="84"/>
-      <c r="C27" s="84"/>
-      <c r="D27" s="84"/>
-      <c r="E27" s="84"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="84"/>
-      <c r="H27" s="85"/>
+      <c r="A27" s="81"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="82"/>
+      <c r="H27" s="83"/>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
-        <v>64</v>
+        <v>196</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E28" s="32" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="F28" s="33" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="H28" s="34" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="G29" s="21" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="83"/>
-      <c r="B30" s="84"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="84"/>
-      <c r="E30" s="84"/>
-      <c r="F30" s="84"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="85"/>
+      <c r="A30" s="81"/>
+      <c r="B30" s="82"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="83"/>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
-        <v>65</v>
+        <v>197</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="F31" s="33" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="G31" s="32" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="H31" s="34" t="s">
-        <v>38</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="F32" s="23" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="H32" s="24" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="83"/>
-      <c r="B33" s="84"/>
-      <c r="C33" s="84"/>
-      <c r="D33" s="84"/>
-      <c r="E33" s="84"/>
-      <c r="F33" s="84"/>
-      <c r="G33" s="84"/>
-      <c r="H33" s="85"/>
+      <c r="A33" s="81"/>
+      <c r="B33" s="82"/>
+      <c r="C33" s="82"/>
+      <c r="D33" s="82"/>
+      <c r="E33" s="82"/>
+      <c r="F33" s="82"/>
+      <c r="G33" s="82"/>
+      <c r="H33" s="83"/>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
-        <v>66</v>
+        <v>198</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E34" s="32" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="F34" s="33" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="G34" s="32" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="H34" s="34" t="s">
-        <v>39</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="G35" s="21" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="H35" s="24" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="89"/>
-      <c r="B36" s="90"/>
-      <c r="C36" s="90"/>
-      <c r="D36" s="90"/>
-      <c r="E36" s="90"/>
-      <c r="F36" s="90"/>
-      <c r="G36" s="90"/>
-      <c r="H36" s="91"/>
+      <c r="A36" s="84"/>
+      <c r="B36" s="85"/>
+      <c r="C36" s="85"/>
+      <c r="D36" s="85"/>
+      <c r="E36" s="85"/>
+      <c r="F36" s="85"/>
+      <c r="G36" s="85"/>
+      <c r="H36" s="86"/>
     </row>
     <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="35" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="B37" s="36" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="E37" s="37" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="F37" s="38" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="G37" s="37" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="H37" s="39" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="40" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="D38" s="41" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="E38" s="41" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="F38" s="42" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="G38" s="41" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="H38" s="43" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="83"/>
-      <c r="B39" s="84"/>
-      <c r="C39" s="84"/>
-      <c r="D39" s="84"/>
-      <c r="E39" s="84"/>
-      <c r="F39" s="84"/>
-      <c r="G39" s="84"/>
-      <c r="H39" s="85"/>
+      <c r="A39" s="81"/>
+      <c r="B39" s="82"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="82"/>
+      <c r="F39" s="82"/>
+      <c r="G39" s="82"/>
+      <c r="H39" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A12:H12"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="A18:H18"/>
     <mergeCell ref="A21:H21"/>
@@ -3130,11 +3121,6 @@
     <mergeCell ref="A30:H30"/>
     <mergeCell ref="A33:H33"/>
     <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A12:H12"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3146,8 +3132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E748FC68-B45F-4508-A7C1-F644815860A2}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3164,707 +3150,702 @@
   <sheetData>
     <row r="1" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="C1" s="47" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="G1" s="47" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="H1" s="48" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="95" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="97"/>
+      <c r="A2" s="90" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="92"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="58" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="B3" s="59">
         <v>44364</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E3" s="60" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F3" s="61" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G3" s="60"/>
       <c r="H3" s="62"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="92"/>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="94"/>
+      <c r="A4" s="93"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="95"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="58" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B5" s="59">
         <v>44364</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F5" s="61" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G5" s="60"/>
       <c r="H5" s="62"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="92"/>
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="94"/>
+      <c r="A6" s="93"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="95"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="63" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="B7" s="64">
         <v>44364</v>
       </c>
       <c r="C7" s="65" t="s">
-        <v>57</v>
+        <v>189</v>
       </c>
       <c r="D7" s="44" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="E7" s="66" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F7" s="67" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G7" s="66"/>
       <c r="H7" s="68"/>
     </row>
-    <row r="8" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="49" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="B8" s="50">
         <v>44364</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D8" s="55" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F8" s="53" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G8" s="52"/>
       <c r="H8" s="54"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="92"/>
-      <c r="B9" s="93"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="94"/>
+      <c r="A9" s="93"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="95"/>
     </row>
     <row r="10" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="B10" s="64">
         <v>44364</v>
       </c>
       <c r="C10" s="65" t="s">
-        <v>58</v>
+        <v>190</v>
       </c>
       <c r="D10" s="44" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="E10" s="66" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F10" s="67" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G10" s="66"/>
       <c r="H10" s="68"/>
     </row>
-    <row r="11" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="49" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="B11" s="50">
         <v>44364</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="D11" s="55" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F11" s="53" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G11" s="52"/>
       <c r="H11" s="54"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="92"/>
-      <c r="B12" s="93"/>
-      <c r="C12" s="93"/>
-      <c r="D12" s="93"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="93"/>
-      <c r="G12" s="93"/>
-      <c r="H12" s="94"/>
+      <c r="A12" s="93"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="95"/>
     </row>
     <row r="13" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="B13" s="64">
         <v>44364</v>
       </c>
       <c r="C13" s="65" t="s">
-        <v>59</v>
+        <v>191</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="E13" s="66" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F13" s="67" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G13" s="66"/>
       <c r="H13" s="68"/>
     </row>
-    <row r="14" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="49" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="B14" s="50">
         <v>44364</v>
       </c>
       <c r="C14" s="51" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="D14" s="55" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="E14" s="52" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F14" s="53" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G14" s="52"/>
       <c r="H14" s="54"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="92"/>
-      <c r="B15" s="93"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="93"/>
-      <c r="G15" s="93"/>
-      <c r="H15" s="94"/>
+      <c r="A15" s="93"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="95"/>
     </row>
     <row r="16" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="69" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="B16" s="64">
         <v>44364</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>60</v>
+        <v>192</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="E16" s="66" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F16" s="67" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G16" s="66"/>
       <c r="H16" s="68"/>
     </row>
-    <row r="17" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="56" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="B17" s="50">
         <v>44364</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="D17" s="55" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="E17" s="52" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F17" s="53" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G17" s="52"/>
       <c r="H17" s="54"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="92"/>
-      <c r="B18" s="93"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="94"/>
+      <c r="A18" s="93"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="94"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="95"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="69" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="B19" s="64">
         <v>44364</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>61</v>
+        <v>193</v>
       </c>
       <c r="D19" s="44" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="E19" s="66" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F19" s="67" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G19" s="66"/>
       <c r="H19" s="68"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="56" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="B20" s="50">
         <v>44364</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D20" s="55" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="E20" s="52" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F20" s="53" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G20" s="52"/>
       <c r="H20" s="54"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="92"/>
-      <c r="B21" s="93"/>
-      <c r="C21" s="93"/>
-      <c r="D21" s="93"/>
-      <c r="E21" s="93"/>
-      <c r="F21" s="93"/>
-      <c r="G21" s="93"/>
-      <c r="H21" s="94"/>
+      <c r="A21" s="93"/>
+      <c r="B21" s="94"/>
+      <c r="C21" s="94"/>
+      <c r="D21" s="94"/>
+      <c r="E21" s="94"/>
+      <c r="F21" s="94"/>
+      <c r="G21" s="94"/>
+      <c r="H21" s="95"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="69" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="B22" s="64">
         <v>44364</v>
       </c>
       <c r="C22" s="65" t="s">
-        <v>62</v>
+        <v>194</v>
       </c>
       <c r="D22" s="44" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="E22" s="66" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F22" s="67" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G22" s="66"/>
       <c r="H22" s="68"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="56" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="B23" s="50">
         <v>44364</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="D23" s="55" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="E23" s="52" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F23" s="53" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G23" s="52"/>
       <c r="H23" s="54"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="92"/>
-      <c r="B24" s="93"/>
-      <c r="C24" s="93"/>
-      <c r="D24" s="93"/>
-      <c r="E24" s="93"/>
-      <c r="F24" s="93"/>
-      <c r="G24" s="93"/>
-      <c r="H24" s="94"/>
+      <c r="A24" s="93"/>
+      <c r="B24" s="94"/>
+      <c r="C24" s="94"/>
+      <c r="D24" s="94"/>
+      <c r="E24" s="94"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="94"/>
+      <c r="H24" s="95"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="69" t="s">
-        <v>185</v>
-      </c>
-      <c r="B25" s="70">
+        <v>164</v>
+      </c>
+      <c r="B25" s="96">
         <v>44364</v>
       </c>
       <c r="C25" s="65" t="s">
-        <v>63</v>
+        <v>195</v>
       </c>
       <c r="D25" s="44" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="E25" s="66" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F25" s="67" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G25" s="66"/>
       <c r="H25" s="68"/>
     </row>
-    <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="56" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="B26" s="50">
         <v>44364</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="D26" s="55" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="E26" s="52" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F26" s="53" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G26" s="52"/>
       <c r="H26" s="54"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="92"/>
-      <c r="B27" s="93"/>
-      <c r="C27" s="93"/>
-      <c r="D27" s="93"/>
-      <c r="E27" s="93"/>
-      <c r="F27" s="93"/>
-      <c r="G27" s="93"/>
-      <c r="H27" s="94"/>
+      <c r="A27" s="93"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="94"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="94"/>
+      <c r="H27" s="95"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="69" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="B28" s="64">
         <v>44364</v>
       </c>
       <c r="C28" s="65" t="s">
-        <v>64</v>
+        <v>196</v>
       </c>
       <c r="D28" s="44" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="E28" s="66" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F28" s="67" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G28" s="66"/>
       <c r="H28" s="68"/>
     </row>
-    <row r="29" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="56" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="B29" s="50">
         <v>44364</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="D29" s="55" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="E29" s="52" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F29" s="53" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G29" s="52"/>
       <c r="H29" s="54"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="92"/>
-      <c r="B30" s="93"/>
-      <c r="C30" s="93"/>
-      <c r="D30" s="93"/>
-      <c r="E30" s="93"/>
-      <c r="F30" s="93"/>
-      <c r="G30" s="93"/>
-      <c r="H30" s="94"/>
+      <c r="A30" s="93"/>
+      <c r="B30" s="94"/>
+      <c r="C30" s="94"/>
+      <c r="D30" s="94"/>
+      <c r="E30" s="94"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="94"/>
+      <c r="H30" s="95"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="69" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="B31" s="64">
         <v>44364</v>
       </c>
       <c r="C31" s="65" t="s">
-        <v>65</v>
+        <v>197</v>
       </c>
       <c r="D31" s="44" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="E31" s="66" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F31" s="67" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G31" s="66"/>
       <c r="H31" s="68"/>
     </row>
-    <row r="32" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="56" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="B32" s="50">
         <v>44364</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="D32" s="55" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="E32" s="52" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F32" s="53" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G32" s="52"/>
       <c r="H32" s="54"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="92"/>
-      <c r="B33" s="93"/>
-      <c r="C33" s="93"/>
-      <c r="D33" s="93"/>
-      <c r="E33" s="93"/>
-      <c r="F33" s="93"/>
-      <c r="G33" s="93"/>
-      <c r="H33" s="94"/>
+      <c r="A33" s="93"/>
+      <c r="B33" s="94"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="94"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="94"/>
+      <c r="G33" s="94"/>
+      <c r="H33" s="95"/>
     </row>
     <row r="34" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="69" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="B34" s="64">
         <v>44364</v>
       </c>
       <c r="C34" s="65" t="s">
-        <v>66</v>
+        <v>198</v>
       </c>
       <c r="D34" s="44" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="E34" s="66" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F34" s="67" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G34" s="66"/>
       <c r="H34" s="68"/>
     </row>
-    <row r="35" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="56" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="B35" s="50">
         <v>44364</v>
       </c>
       <c r="C35" s="51" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="D35" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="E35" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="F35" s="53" t="s">
         <v>174</v>
-      </c>
-      <c r="E35" s="52" t="s">
-        <v>151</v>
-      </c>
-      <c r="F35" s="53" t="s">
-        <v>195</v>
       </c>
       <c r="G35" s="52"/>
       <c r="H35" s="54"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="92"/>
-      <c r="B36" s="93"/>
-      <c r="C36" s="93"/>
-      <c r="D36" s="93"/>
-      <c r="E36" s="93"/>
-      <c r="F36" s="93"/>
-      <c r="G36" s="93"/>
-      <c r="H36" s="94"/>
+      <c r="A36" s="93"/>
+      <c r="B36" s="94"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="94"/>
+      <c r="E36" s="94"/>
+      <c r="F36" s="94"/>
+      <c r="G36" s="94"/>
+      <c r="H36" s="95"/>
     </row>
     <row r="37" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="69" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="B37" s="64">
         <v>44364</v>
       </c>
       <c r="C37" s="65" t="s">
-        <v>128</v>
-      </c>
-      <c r="D37" s="71" t="s">
-        <v>41</v>
+        <v>107</v>
+      </c>
+      <c r="D37" s="70" t="s">
+        <v>30</v>
       </c>
       <c r="E37" s="66" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F37" s="67" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G37" s="66"/>
       <c r="H37" s="68"/>
     </row>
-    <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="56" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="B38" s="50">
         <v>44364</v>
       </c>
       <c r="C38" s="51" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="D38" s="57" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="E38" s="52" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F38" s="53" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G38" s="52"/>
       <c r="H38" s="54"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="92"/>
-      <c r="B39" s="93"/>
-      <c r="C39" s="93"/>
-      <c r="D39" s="93"/>
-      <c r="E39" s="93"/>
-      <c r="F39" s="93"/>
-      <c r="G39" s="93"/>
-      <c r="H39" s="94"/>
+      <c r="A39" s="93"/>
+      <c r="B39" s="94"/>
+      <c r="C39" s="94"/>
+      <c r="D39" s="94"/>
+      <c r="E39" s="94"/>
+      <c r="F39" s="94"/>
+      <c r="G39" s="94"/>
+      <c r="H39" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A12:H12"/>
     <mergeCell ref="A33:H33"/>
     <mergeCell ref="A36:H36"/>
     <mergeCell ref="A39:H39"/>
@@ -3874,6 +3855,11 @@
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A12:H12"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>